<commit_message>
userinfo form done, next to mod userinfo and password
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAADB92-4D76-42DF-8F1D-94E71871E3C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E234B8-CBD1-4452-ABF4-DEC36D751CAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14055" yWindow="1830" windowWidth="17055" windowHeight="12465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11475" yWindow="540" windowWidth="17055" windowHeight="12465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Client存储用户信息，并检查用户是否已完善个人详细信息，若没完成，对话框提示，跳转页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>必要信息包括：</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -128,14 +124,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>组织信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Client存储用户信息，并检查用户是否已完善个人详细信息，若没完成，跳转个人信息页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>detailed_info_done</t>
-  </si>
-  <si>
-    <t>组织信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>若未完成，是否存储token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路由before，根据detailed_info_done控制跳转</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -246,7 +247,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -298,7 +299,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -607,7 +608,7 @@
   <dimension ref="B1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -624,45 +625,45 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
done - user info page, next - account setting page
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23E234B8-CBD1-4452-ABF4-DEC36D751CAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B41055-7F31-4B6E-8E6C-D0F9DFBA8475}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="540" windowWidth="17055" windowHeight="12465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10395" yWindow="2625" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="注册" sheetId="1" r:id="rId1"/>
     <sheet name="登录" sheetId="2" r:id="rId2"/>
+    <sheet name="用户设置" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,51 +93,109 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>登录成功</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Server反馈必要的用户信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>必要信息包括：</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>uid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>phone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>active</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>组织信息</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Client存储用户信息，并检查用户是否已完善个人详细信息，若没完成，跳转个人信息页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>detailed_info_done</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>路由before，根据detailed_info_done控制跳转</t>
+    <t>client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>server</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api - requestUserInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db api - get_user_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reposonse client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>controller - Users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method - request_user_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收到response</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向server request用户信息，页面等待加载</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收到response，取消页面加载</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户信息Tab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api - updateUserInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>账号管理Tab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api - updateEmail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api - updatePassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api - updatePhone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method - update_user_info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>detailed_info_done 置1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api -store - Login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method - login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db api - login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功</t>
+  </si>
+  <si>
+    <t>store {active, detailed_info}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>detailed_info_done = 0 跳转至“用户设置”页面</t>
+  </si>
+  <si>
+    <t>保存Token</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{active, detailed_info_done}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -183,8 +242,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -605,74 +667,193 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D3D4B6-D229-4FBC-A736-8E613F9C066A}">
-  <dimension ref="B1:E12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="30.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43573</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FD2C70-64CE-4F76-9328-7F7B5831545C}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43573</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working on update user settings
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B41055-7F31-4B6E-8E6C-D0F9DFBA8475}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="2625" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10395" yWindow="2625" windowWidth="21600" windowHeight="11505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="注册" sheetId="1" r:id="rId1"/>
     <sheet name="登录" sheetId="2" r:id="rId2"/>
     <sheet name="用户设置" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -137,14 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>api - updateUserInfo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>账号管理Tab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>api - updateEmail</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -157,10 +143,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>method - update_user_info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>detailed_info_done 置1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -196,14 +178,30 @@
   </si>
   <si>
     <t>{active, detailed_info_done}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api - updateUserProfile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method - update_user_profile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码Tab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method - update_password</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,7 +307,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -361,7 +359,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -555,33 +553,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="3:9">
       <c r="I1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:9">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -592,17 +590,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:9">
       <c r="I3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:9">
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:9">
       <c r="F5" t="s">
         <v>3</v>
       </c>
@@ -610,17 +608,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:9">
       <c r="F6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:9">
       <c r="F7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:9">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -628,32 +626,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:9">
       <c r="C11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:9">
       <c r="F13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:9">
       <c r="F14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:9">
       <c r="C16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:6">
       <c r="F18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:6">
       <c r="F19" t="s">
         <v>5</v>
       </c>
@@ -666,21 +664,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D3D4B6-D229-4FBC-A736-8E613F9C066A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="30.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="C1" t="s">
         <v>16</v>
       </c>
@@ -688,61 +686,61 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>43573</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="D5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="H6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="C8" t="s">
         <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="C9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="D10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="D11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="D12" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -752,14 +750,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16FD2C70-64CE-4F76-9328-7F7B5831545C}">
-  <dimension ref="A1:H18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.75" bestFit="1" customWidth="1"/>
@@ -768,7 +766,7 @@
     <col min="8" max="8" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="C1" t="s">
         <v>16</v>
       </c>
@@ -776,7 +774,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>43573</v>
       </c>
@@ -787,7 +785,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="D5" t="s">
         <v>18</v>
       </c>
@@ -795,22 +793,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="H6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="C8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="C11" t="s">
         <v>26</v>
       </c>
@@ -818,37 +816,43 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="H13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4">
+      <c r="D19" t="s">
         <v>27</v>
-      </c>
-      <c r="G12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done update password, working on update email
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359EB7F0-A449-4574-BB0C-CF80290433B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10395" yWindow="2625" windowWidth="21600" windowHeight="11505" activeTab="2"/>
+    <workbookView xWindow="11475" yWindow="540" windowWidth="17055" windowHeight="12465" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="注册" sheetId="1" r:id="rId1"/>
@@ -12,8 +18,8 @@
     <sheet name="用户设置" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,10 +133,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>用户信息Tab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>api - updateEmail</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -189,19 +191,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>密码Tab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>method - update_password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建token，包含phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功，清空表单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>邮箱 Tab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码 Tab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户信息 Tab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method - update_email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>token中取出phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以phone检索user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核对email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核对验证码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核对旧密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新密码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功，清空表单，更新组件data.email</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +266,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -240,11 +302,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -307,7 +372,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -359,7 +424,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -553,33 +618,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="3:9">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -590,17 +655,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="3:9">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="3:9">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:9">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F5" t="s">
         <v>3</v>
       </c>
@@ -608,17 +673,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:9">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:9">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:9">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -626,32 +691,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:9">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:9">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="3:9">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="3:9">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
         <v>5</v>
       </c>
@@ -664,21 +729,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="30.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>16</v>
       </c>
@@ -686,78 +751,84 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43573</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="H6" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="C9" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="D11" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="D12" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.75" bestFit="1" customWidth="1"/>
@@ -766,7 +837,7 @@
     <col min="8" max="8" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>16</v>
       </c>
@@ -774,7 +845,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43573</v>
       </c>
@@ -785,7 +856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>18</v>
       </c>
@@ -793,66 +864,125 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43574</v>
+      </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
         <v>40</v>
       </c>
-      <c r="G12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
         <v>28</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done update email, next update phone
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359EB7F0-A449-4574-BB0C-CF80290433B9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D52532F-3F63-43F9-8D84-BE6B09357E2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="540" windowWidth="17055" windowHeight="12465" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3135" yWindow="2490" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="注册" sheetId="1" r:id="rId1"/>
-    <sheet name="登录" sheetId="2" r:id="rId2"/>
-    <sheet name="用户设置" sheetId="3" r:id="rId3"/>
+    <sheet name="Store" sheetId="4" r:id="rId1"/>
+    <sheet name="注册" sheetId="1" r:id="rId2"/>
+    <sheet name="登录" sheetId="2" r:id="rId3"/>
+    <sheet name="用户设置" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="63">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,10 +228,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>核对email</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>更新email</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -248,6 +245,38 @@
   </si>
   <si>
     <t>成功，清空表单，更新组件data.email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api-requestCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核对旧email</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>手机号 Tab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更改手机号，需更新Token，因为，Token中Claim 手机号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logout</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -625,6 +654,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141386CE-6611-4B1D-86BC-C2C2ACDF9D64}">
+  <dimension ref="B1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:I19"/>
   <sheetViews>
@@ -728,12 +794,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -820,12 +886,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -921,12 +987,12 @@
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.2">
@@ -944,44 +1010,59 @@
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
         <v>26</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G24" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G24" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D31" t="s">
+      <c r="G28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
working on Gen start  log
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DE5D79-5637-44F4-8217-2CA0E61A99C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D418E06-AB76-46E4-9DD7-8E99D7DC65EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="1665" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="795" yWindow="135" windowWidth="17055" windowHeight="12465" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="注册" sheetId="1" r:id="rId3"/>
     <sheet name="登录" sheetId="2" r:id="rId4"/>
     <sheet name="用户设置" sheetId="3" r:id="rId5"/>
+    <sheet name="机组启停记录" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -327,6 +328,102 @@
   </si>
   <si>
     <t>路由控制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机组编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>启动时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记录人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>停止时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>db</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电厂编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改、删除，限制录入人操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>excel文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中文姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>page-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>停止标志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1-未停止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2-已停止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login后 store用户哪些信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -454,7 +551,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -506,7 +603,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -708,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5285995A-95A9-432A-A76E-84A20180A172}">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A2:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -728,6 +825,17 @@
       </c>
       <c r="C2" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>43577</v>
+      </c>
+      <c r="C3" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1209,4 +1317,147 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D69B08E-BFAA-4F63-9B9E-AA36DC360167}">
+  <dimension ref="A3:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43577</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F6" s="2"/>
+      <c r="I6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
before remove org_dept_level from user db
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6590A33D-049B-46EC-8E5D-CDB70A511CF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="135" windowWidth="17055" windowHeight="12465" activeTab="2"/>
+    <workbookView xWindow="10500" yWindow="2040" windowWidth="17055" windowHeight="12465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -16,8 +22,8 @@
     <sheet name="机组启停记录" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="118">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -402,18 +408,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>停止标志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-未停止</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2-已停止</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Login后 store用户哪些信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -447,14 +441,98 @@
   </si>
   <si>
     <t>苏家河口电厂对象编号 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择机组编号，向server查找记录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api-getGenStartLog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method -get_gen_start_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>controller - Devices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行标志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRunning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRunning = TRUE，机组运行，回应启动时间（不可编辑），要求填写停止时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRunning = FALSE，机组停止，填写启动时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>para</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stationIdx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>genIdx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面加载，识别用户，获取stationIdx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户登录成功，未点击退出关闭浏览器或窗口，Token未过期，再打开网页，store的用户信息是否丢失</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>查找</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>最后一条</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>记录</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,6 +553,14 @@
       <color rgb="FFFF0000"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -820,26 +906,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -850,7 +936,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -858,7 +944,18 @@
         <v>43577</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>43578</v>
+      </c>
+      <c r="C4" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -868,16 +965,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="3:9">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>58</v>
       </c>
@@ -885,7 +982,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="3:9">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>57</v>
       </c>
@@ -893,7 +990,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="3:9">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>61</v>
       </c>
@@ -908,39 +1005,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43578</v>
       </c>
       <c r="C2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="C3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="C5" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -950,26 +1047,26 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="3:9">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -980,17 +1077,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="3:9">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="3:9">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:9">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F5" t="s">
         <v>3</v>
       </c>
@@ -998,17 +1095,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="3:9">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:9">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:9">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -1016,32 +1113,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:9">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:9">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="3:9">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="3:9">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
         <v>5</v>
       </c>
@@ -1054,21 +1151,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="30.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>16</v>
       </c>
@@ -1076,7 +1173,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43573</v>
       </c>
@@ -1087,7 +1184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>31</v>
       </c>
@@ -1095,22 +1192,22 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G7" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>23</v>
       </c>
@@ -1118,22 +1215,22 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>67</v>
       </c>
@@ -1146,14 +1243,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
@@ -1163,7 +1260,7 @@
     <col min="8" max="8" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>16</v>
       </c>
@@ -1171,7 +1268,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43573</v>
       </c>
@@ -1182,7 +1279,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>18</v>
       </c>
@@ -1190,22 +1287,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43574</v>
       </c>
@@ -1216,7 +1313,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>38</v>
       </c>
@@ -1224,12 +1321,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>44</v>
       </c>
@@ -1237,7 +1334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>27</v>
       </c>
@@ -1245,22 +1342,22 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="3:8">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
       <c r="G17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="3:8">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
       <c r="G18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="3:8">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="3:8">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>43</v>
       </c>
@@ -1268,7 +1365,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="3:8">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>54</v>
       </c>
@@ -1276,7 +1373,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="3:8">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D23" s="3" t="s">
         <v>71</v>
       </c>
@@ -1284,10 +1381,10 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="3:8">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D24" s="3"/>
     </row>
-    <row r="25" spans="3:8">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>26</v>
       </c>
@@ -1295,47 +1392,47 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="3:8">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="3:8">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
       <c r="H27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="3:8">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="3:8">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="3:8">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="3:8">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D34" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43575</v>
       </c>
@@ -1343,12 +1440,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D36" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>28</v>
       </c>
@@ -1356,7 +1453,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D38" s="3" t="s">
         <v>70</v>
       </c>
@@ -1364,12 +1461,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H39" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
         <v>69</v>
       </c>
@@ -1385,35 +1482,35 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>43578</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43577</v>
       </c>
@@ -1421,12 +1518,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E5" t="s">
         <v>79</v>
@@ -1435,38 +1532,35 @@
         <v>78</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D6" s="2" t="s">
         <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D7" s="2"/>
-      <c r="G7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>86</v>
       </c>
@@ -1480,7 +1574,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>87</v>
       </c>
@@ -1488,7 +1582,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
         <v>83</v>
       </c>
@@ -1499,12 +1593,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="3:6">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F17" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="3:6">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>92</v>
       </c>
@@ -1512,12 +1606,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="3:6">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="3:6">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>82</v>
       </c>
@@ -1528,9 +1622,69 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="3:6">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D22" s="2" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43578</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>115</v>
+      </c>
+      <c r="H27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+      <c r="I29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="J30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>112</v>
+      </c>
+      <c r="J31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made beforerouter, rmv org_dept_lvl from user db
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D312509-0D69-45A5-A8F8-687E25C62364}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBFE256-0FB3-46B0-9931-21EF77D7BDF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="975" yWindow="2865" windowWidth="17055" windowHeight="12465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6195" yWindow="1665" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="131">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -540,23 +540,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Client采用cookie方式存储token，设置有效期30minutes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>浏览器关闭或超期，cookie失效</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关闭浏览器或超期，cookie失效</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>关闭浏览器窗口，vue store 销毁</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用户登录成功，未点击退出，只关闭浏览器的窗口，Token未过期，再打开网页，store中信息销毁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Client采用cookie方式存储token，采用js-cookie包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建cookie时，未set expires，关闭浏览器，cookie被销毁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建cookie时，set expires，关闭浏览器，cookie不会被销毁，直到过期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关闭或刷新浏览器窗口，vue store 销毁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cookie 设置exp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刷新窗口-有cookie，无store</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次登录-有cookie，无store</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关闭浏览器-有cookie，无store</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首次打开页面-无cookie，无store</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -968,10 +988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1009,17 +1029,27 @@
         <v>43578</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C5" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C7" s="5" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1100,10 +1130,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1111,7 +1141,7 @@
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43578</v>
       </c>
@@ -1119,34 +1149,64 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done router control, working on Gen_start_log
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBFE256-0FB3-46B0-9931-21EF77D7BDF6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910FA237-A970-4C2F-998A-9BD17D87EBC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="1665" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12225" yWindow="2685" windowWidth="17055" windowHeight="12465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
     <sheet name="Store" sheetId="4" r:id="rId2"/>
     <sheet name="全局" sheetId="7" r:id="rId3"/>
-    <sheet name="注册" sheetId="1" r:id="rId4"/>
-    <sheet name="登录" sheetId="2" r:id="rId5"/>
-    <sheet name="用户设置" sheetId="3" r:id="rId6"/>
-    <sheet name="机组启停记录" sheetId="6" r:id="rId7"/>
+    <sheet name="路由" sheetId="8" r:id="rId4"/>
+    <sheet name="注册" sheetId="1" r:id="rId5"/>
+    <sheet name="登录" sheetId="2" r:id="rId6"/>
+    <sheet name="用户设置" sheetId="3" r:id="rId7"/>
+    <sheet name="机组启停记录" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="152">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -273,10 +274,6 @@
   </si>
   <si>
     <t>logout</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{active, detailed_info}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -577,6 +574,92 @@
   </si>
   <si>
     <t>首次打开页面-无cookie，无store</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>permission.js文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端路由，添加跳转控制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置routerFullList，含所有前端路由项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置whiteList，含无需token的前端路由项</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>访问未定义的前端路由，返回404页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>登录后跳转到之前的页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>permission.js中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login页面，登录成功，若url中有query重定向，路由跳转至指定的path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>this.$router.replace({ path: this.redirect || '/' })</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路由跳转时，将访问路径保存在query中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>next(`/login?redirect=${to.path}`)</t>
+  </si>
+  <si>
+    <t>前端路由列表，怎么识别重置密码url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login成功，store token和user_state，含激活状态和个人信息完成状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>permission.js中，检测store中用户信息空，则携带token向服务器请求</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>permission.js</t>
+  </si>
+  <si>
+    <t>{phone, email, user_profile}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{phone}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{token, active, detailed_info}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/user/setting 页面中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更改用户信息，邮箱后，用store方法GetUserProfile向服务器请求，失败跳转至login页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更改手机号，已要求重新登录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -618,7 +701,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -626,19 +709,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -655,7 +744,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -673,6 +762,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -988,68 +1086,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C8"/>
+  <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>43575</v>
       </c>
-      <c r="C2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>43577</v>
       </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="D3" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
+        <v>43579</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+      <c r="D5" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="1">
         <v>43578</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D6" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C5" s="5" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C6" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C7" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" s="4" t="s">
-        <v>121</v>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43579</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1060,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1071,54 +1195,89 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H1" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="L1" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>57</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>148</v>
+      </c>
+      <c r="L4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>144</v>
+      </c>
+      <c r="L5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>43578</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
         <v>117</v>
       </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+      <c r="D14" t="s">
         <v>118</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E9" t="s">
-        <v>120</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="I15" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1132,7 +1291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1146,67 +1305,67 @@
         <v>43578</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1216,6 +1375,83 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5709F210-9363-48A0-87DA-43FC9D18AB36}">
+  <dimension ref="A3:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43579</v>
+      </c>
+      <c r="C3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C1:I19"/>
   <sheetViews>
@@ -1319,7 +1555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
@@ -1401,7 +1637,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1411,7 +1647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
@@ -1539,15 +1775,15 @@
         <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.2">
       <c r="D23" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.2">
@@ -1598,7 +1834,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1606,12 +1842,12 @@
         <v>43575</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D36" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1619,12 +1855,12 @@
         <v>28</v>
       </c>
       <c r="G37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D38" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H38" t="s">
         <v>47</v>
@@ -1632,15 +1868,15 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1650,7 +1886,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
@@ -1668,12 +1904,12 @@
         <v>43578</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1684,32 +1920,32 @@
         <v>43577</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s">
         <v>77</v>
       </c>
-      <c r="D5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>78</v>
-      </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1720,85 +1956,85 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
         <v>76</v>
       </c>
-      <c r="E14" t="s">
-        <v>77</v>
-      </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
         <v>87</v>
-      </c>
-      <c r="D15" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
         <v>83</v>
       </c>
-      <c r="E16" t="s">
-        <v>84</v>
-      </c>
       <c r="F16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
         <v>92</v>
-      </c>
-      <c r="D18" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>83</v>
-      </c>
-      <c r="E21" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D22" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1806,54 +2042,54 @@
         <v>43578</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
keeping on gen start log
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910FA237-A970-4C2F-998A-9BD17D87EBC8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDD6CE7-03B9-4D61-8334-2AB7350D7D58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12225" yWindow="2685" windowWidth="17055" windowHeight="12465" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="465" windowWidth="15375" windowHeight="10245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="152">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -449,14 +449,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>api-getGenStartLog</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>method -get_gen_start_log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>controller - Devices</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -474,10 +466,6 @@
   </si>
   <si>
     <t>isRunning = FALSE，机组停止，填写启动时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>para</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -662,12 +650,24 @@
     <t>更改手机号，已要求重新登录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>api-getGenStartLastLog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method -gen_start_last_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机组启停记录，如何处理跨月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,6 +715,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -744,7 +752,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -771,6 +779,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1086,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1125,13 +1136,13 @@
         <v>43579</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="D5" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1142,27 +1153,27 @@
         <v>43578</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D7" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D8" s="5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D9" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D10" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1173,7 +1184,18 @@
         <v>43579</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43580</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1186,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1207,7 +1229,7 @@
         <v>59</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1215,28 +1237,28 @@
         <v>57</v>
       </c>
       <c r="L3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1246,12 +1268,12 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I9" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1259,7 +1281,7 @@
         <v>43578</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H13" t="s">
         <v>21</v>
@@ -1267,15 +1289,15 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I15" t="s">
         <v>22</v>
@@ -1325,47 +1347,47 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1392,57 +1414,57 @@
         <v>43579</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1888,10 +1910,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="D19" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1937,7 +1959,7 @@
         <v>77</v>
       </c>
       <c r="G5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1945,7 +1967,7 @@
         <v>90</v>
       </c>
       <c r="G6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2047,15 +2069,15 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I28" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -2063,33 +2085,28 @@
         <v>103</v>
       </c>
       <c r="I29" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="J30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J31" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="F32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F33" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done front page of gen start log, plan to server process  of gen start log
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDD6CE7-03B9-4D61-8334-2AB7350D7D58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3EC2F8-54BD-4D83-91C1-8AADDF2A6AC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="465" windowWidth="15375" windowHeight="10245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="633" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="183">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -449,23 +449,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>controller - Devices</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>运行标志</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>isRunning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>isRunning = TRUE，机组运行，回应启动时间（不可编辑），要求填写停止时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>isRunning = FALSE，机组停止，填写启动时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -660,6 +648,141 @@
   </si>
   <si>
     <t>机组启停记录，如何处理跨月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRunning</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>client时间-Date对象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>server时间-timestamp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>js timestamp有效长度到毫秒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>php time() 有效长度到秒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写入处理，/1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取出处理，*1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面显示控制变量回初始状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求成功</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据isRunning更新页面显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>controller - Device</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向server提交</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>插入新表项，开机时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新最后一条表项，停止时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRunning = 0，机组停止，填写启动时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRunning = 1，机组运行，回应启动时间（不可编辑），要求填写停止时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRunning = 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRunning = 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dateTime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api-logGenStartStop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>method - log_gen_start_last</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交成功</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>提交失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>username</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reset表单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新isRunning=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新isRunning=0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isRunning 来自与db中最后一条记录</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1099,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1136,13 +1259,13 @@
         <v>43579</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="D5" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1153,27 +1276,27 @@
         <v>43578</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D7" s="5" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D8" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D9" s="5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D10" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1184,7 +1307,7 @@
         <v>43579</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1195,7 +1318,7 @@
         <v>43580</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1229,7 +1352,7 @@
         <v>59</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -1237,28 +1360,28 @@
         <v>57</v>
       </c>
       <c r="L3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="L4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="L5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1268,12 +1391,12 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1281,7 +1404,7 @@
         <v>43578</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H13" t="s">
         <v>21</v>
@@ -1289,15 +1412,15 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I15" t="s">
         <v>22</v>
@@ -1347,47 +1470,47 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1414,57 +1537,57 @@
         <v>43579</v>
       </c>
       <c r="C3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1910,10 +2033,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1921,7 +2044,7 @@
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>43578</v>
       </c>
@@ -1929,184 +2052,381 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D5" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>43577</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
+      <c r="H7" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>76</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D8" t="s">
         <v>94</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E8" t="s">
         <v>78</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F8" t="s">
         <v>77</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D6" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D25" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>43578</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>108</v>
+      </c>
+      <c r="H30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G34" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
-        <v>82</v>
-      </c>
-      <c r="E16" t="s">
-        <v>83</v>
-      </c>
-      <c r="F16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D22" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>43578</v>
-      </c>
-      <c r="C26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D27" t="s">
-        <v>111</v>
-      </c>
-      <c r="H27" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I28" t="s">
+      <c r="I34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G35" t="s">
+        <v>107</v>
+      </c>
+      <c r="J35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="J36" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>149</v>
+      </c>
+      <c r="K38" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D29" t="s">
-        <v>103</v>
-      </c>
-      <c r="I29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="E30" t="s">
-        <v>149</v>
-      </c>
-      <c r="J30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F31" t="s">
-        <v>109</v>
-      </c>
-      <c r="J31" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F32" t="s">
-        <v>110</v>
+      <c r="L38" t="s">
+        <v>151</v>
+      </c>
+      <c r="M38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="K39" t="s">
+        <v>153</v>
+      </c>
+      <c r="L39" t="s">
+        <v>153</v>
+      </c>
+      <c r="M39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>161</v>
+      </c>
+      <c r="K40" t="s">
+        <v>154</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G41" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F44" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="49" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G51" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G54" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="F56" t="s">
+        <v>174</v>
+      </c>
+      <c r="I56" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G57" t="s">
+        <v>152</v>
+      </c>
+      <c r="J57" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
+        <v>173</v>
+      </c>
+      <c r="K58" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
+        <v>178</v>
+      </c>
+      <c r="K59" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="J60" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="K61" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="K62" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F65" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="66" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="67" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E67" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="68" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="69" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
done: gen start log on server side
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3EC2F8-54BD-4D83-91C1-8AADDF2A6AC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166B92BD-73BA-4C9A-ADF3-A2E4AC0807BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="633" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="633" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="221">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -783,6 +783,158 @@
   </si>
   <si>
     <t>isRunning 来自与db中最后一条记录</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机组启停记录，如何处理跨月，跨年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计时刻，机组已停机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计时刻，机组未停机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后一条，跨月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一条，跨月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>情况1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首条，最末一条，都没跨月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>情况2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首条跨月，最末一条没跨月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>情况3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首条没跨月，最末条跨月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>情况4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首条，最末条都跨月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找开机时间属于X月的记录 - A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找停机时间属于X月的记录 - B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A=B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A+1=B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A=B+1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A=B，A_id!=B_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>情况1）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不存在情况3，情况4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>情况2）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前时刻 - X月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统计时刻 - Y月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y&gt;X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将来时，不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>情况3）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y&lt;X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y=X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>按月统计，机组开机次数，运行时长</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>停机原因</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建月度统计数据表，定时脚本，每月首日零点更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model-get_gen_start_last_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>model-set_gen_start_last_log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -861,12 +1013,47 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -875,7 +1062,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -905,6 +1092,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1223,7 +1425,7 @@
   <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2033,10 +2235,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="J82" sqref="J82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2044,7 +2246,7 @@
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>43578</v>
       </c>
@@ -2052,15 +2254,15 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>155</v>
       </c>
@@ -2068,7 +2270,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D5" s="2" t="s">
         <v>157</v>
       </c>
@@ -2076,360 +2278,572 @@
         <v>158</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D6" s="2"/>
       <c r="H6" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>43577</v>
-      </c>
-      <c r="C7" t="s">
-        <v>79</v>
-      </c>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D7" s="2"/>
       <c r="H7" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
       <c r="C8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43583</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" t="s">
         <v>76</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>94</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F9" t="s">
         <v>78</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G9" t="s">
         <v>77</v>
       </c>
-      <c r="G8" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="H9" t="s">
+        <v>217</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D9" s="2" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>97</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>74</v>
-      </c>
+      <c r="F13" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
         <v>86</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D19" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
         <v>82</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>83</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F20" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
         <v>91</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
         <v>81</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>82</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D25" s="2" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D26" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
         <v>43578</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D30" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
         <v>108</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D32">
+    <row r="33" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D33">
         <v>1</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E33" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="F33" t="s">
+    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
         <v>146</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I34" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="34" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="G34" t="s">
-        <v>106</v>
-      </c>
-      <c r="I34" t="s">
-        <v>109</v>
+      <c r="L34" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="4:13" x14ac:dyDescent="0.2">
       <c r="G35" t="s">
+        <v>106</v>
+      </c>
+      <c r="I35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G36" t="s">
         <v>107</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J36" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="J36" t="s">
+    <row r="37" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="J38" t="s">
+    <row r="39" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
         <v>149</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K39" t="s">
         <v>150</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L39" t="s">
         <v>151</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M39" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="K39" t="s">
+    <row r="40" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="K40" t="s">
         <v>153</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L40" t="s">
         <v>153</v>
       </c>
-      <c r="M39">
+      <c r="M40">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="F40" t="s">
+    <row r="41" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
         <v>161</v>
       </c>
-      <c r="K40" t="s">
+      <c r="K41" t="s">
         <v>154</v>
       </c>
-      <c r="M40">
+      <c r="M41">
         <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="G41" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="42" spans="4:13" x14ac:dyDescent="0.2">
       <c r="G42" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G43" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="44" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="F44" t="s">
+    <row r="45" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="F45" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="G45" t="s">
+    <row r="46" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="G46" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="4:13" x14ac:dyDescent="0.2">
-      <c r="D48">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>43581</v>
+      </c>
+      <c r="D49">
         <v>2</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="49" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F49" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F50" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="50" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F50" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F51" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="51" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G51" t="s">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G52" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="53" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F53" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F54" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="54" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G54" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G55" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="56" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="F56" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F57" t="s">
         <v>174</v>
       </c>
-      <c r="I56" t="s">
+      <c r="I57" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="57" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G57" t="s">
+      <c r="L57" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G58" t="s">
         <v>152</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J58" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G58" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G59" t="s">
         <v>173</v>
       </c>
-      <c r="K58" t="s">
+      <c r="K59" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="G59" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G60" t="s">
         <v>178</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K60" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="60" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="J60" t="s">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J61" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="61" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="K61" t="s">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K62" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="62" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="K62" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K63" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="64" spans="5:11" x14ac:dyDescent="0.2">
-      <c r="E64" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="F65" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="F66" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E67" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="F68" t="s">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="F69" t="s">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
         <v>162</v>
       </c>
     </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C73" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C75" s="9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>43583</v>
+      </c>
+      <c r="D80" s="12">
+        <v>2</v>
+      </c>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13">
+        <v>3</v>
+      </c>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13">
+        <v>4</v>
+      </c>
+      <c r="I80" s="14"/>
+    </row>
+    <row r="81" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="L81" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="E82" s="11"/>
+      <c r="F82" s="10"/>
+      <c r="L82" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D84" t="s">
+        <v>186</v>
+      </c>
+      <c r="E84" t="s">
+        <v>190</v>
+      </c>
+      <c r="L84" t="s">
+        <v>192</v>
+      </c>
+      <c r="M84" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="85" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D85" t="s">
+        <v>187</v>
+      </c>
+      <c r="E85" t="s">
+        <v>191</v>
+      </c>
+      <c r="M85" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="L86" t="s">
+        <v>194</v>
+      </c>
+      <c r="M86" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="M87" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="88" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="L88" t="s">
+        <v>196</v>
+      </c>
+      <c r="M88" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="89" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D89" s="12">
+        <v>12</v>
+      </c>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13">
+        <v>1</v>
+      </c>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13">
+        <v>2</v>
+      </c>
+      <c r="I89" s="14"/>
+      <c r="M89" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="90" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="L90" t="s">
+        <v>198</v>
+      </c>
+      <c r="M90" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="91" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="E91" s="11"/>
+      <c r="F91" s="10"/>
+      <c r="M91" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="93" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>188</v>
+      </c>
+      <c r="E93" t="s">
+        <v>190</v>
+      </c>
+      <c r="L93" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="94" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="D94" t="s">
+        <v>189</v>
+      </c>
+      <c r="E94" t="s">
+        <v>191</v>
+      </c>
+      <c r="L94" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="96" spans="4:13" x14ac:dyDescent="0.2">
+      <c r="L96" t="s">
+        <v>206</v>
+      </c>
+      <c r="M96" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="97" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="M97" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="99" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L99" t="s">
+        <v>208</v>
+      </c>
+      <c r="M99" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="100" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="M100" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="102" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L102" t="s">
+        <v>213</v>
+      </c>
+      <c r="M102" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="103" spans="12:13" x14ac:dyDescent="0.2">
+      <c r="L103" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="H89:I89"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
mod server for station
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166B92BD-73BA-4C9A-ADF3-A2E4AC0807BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FC9523-9256-42D3-8182-B17CCB4237D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="633" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="465" windowWidth="15375" windowHeight="10245" tabRatio="633" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="244">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -935,6 +935,97 @@
   </si>
   <si>
     <t>model-set_gen_start_last_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电厂内的单元创建数据表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后端路由，作为API接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端路由，控制页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有站点的Controller相同，构造函数中，根据站点ID，选择连接对应的站点DB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>页面内容划分，建议采用嵌套路由</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对象划分层次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>controller按模块划分，如用户，设备，命名添加复数s结尾，如Users，Generators</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Server目录结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>application\controllers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generators.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api-query_start_last_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api-post_start_stop_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>application\third_party\generator\models</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Generator_model.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_start_last_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>set_start_last_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>application\third_party\station\config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>station_config.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>application\third_party\station\language\zh_cn</t>
+  </si>
+  <si>
+    <t>station_lang.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>站点-在Db中体现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发电机-在db的table中，controller中体现</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1636,10 +1727,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:D16"/>
+  <dimension ref="A2:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1715,6 +1806,104 @@
         <v>122</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43583</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C20" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E25" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>241</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1723,10 +1912,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5709F210-9363-48A0-87DA-43FC9D18AB36}">
-  <dimension ref="A3:E14"/>
+  <dimension ref="A3:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1790,6 +1979,34 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43583</v>
+      </c>
+      <c r="C17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2237,8 +2454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="J82" sqref="J82"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
mod files structure of client and server
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FC9523-9256-42D3-8182-B17CCB4237D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9DD97D-7B69-4602-8F0E-6091B2360F7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="465" windowWidth="15375" windowHeight="10245" tabRatio="633" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="255" windowWidth="15375" windowHeight="10245" tabRatio="633" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="258">
   <si>
     <t>Client</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1026,6 +1026,62 @@
   </si>
   <si>
     <t>发电机-在db的table中，controller中体现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>routers匹配：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端路由</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api靠前</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>前端路由靠后</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Client目录结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>client\src\views\station\generator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_stop_log.vue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>client\src\api\station</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>generator.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>client\src\utils</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>station.js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site.com/generator/start_stop_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api-/generators/query_start_last_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>api-/generators/post_start_stop_log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1727,10 +1783,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:E43"/>
+  <dimension ref="A2:E59"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1904,6 +1960,61 @@
         <v>241</v>
       </c>
     </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>255</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1912,10 +2023,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5709F210-9363-48A0-87DA-43FC9D18AB36}">
-  <dimension ref="A3:E22"/>
+  <dimension ref="A3:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1981,7 +2092,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43583</v>
       </c>
@@ -1989,23 +2100,38 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D22" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
         <v>225</v>
       </c>
     </row>

</xml_diff>

<commit_message>
on gen start history
</commit_message>
<xml_diff>
--- a/worknotes.xlsx
+++ b/worknotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\www\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D74F032-40C4-4A62-B59F-427DAC6F41C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AC9573-0136-4E99-9B7E-D3B1967F13ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="390" windowWidth="15375" windowHeight="10245" tabRatio="633" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6195" yWindow="1665" windowWidth="21600" windowHeight="11505" tabRatio="633" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TODO" sheetId="5" r:id="rId1"/>
@@ -1073,15 +1073,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>site.com/generator/start_stop_log</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>api-/generators/query_start_last_log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>api-/generators/post_start_stop_log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>site.com/generator/start_stop/log</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1572,7 +1572,7 @@
   <dimension ref="A2:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1785,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1987,12 +1987,12 @@
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.2">
       <c r="E53" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.2">
@@ -2012,7 +2012,7 @@
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.2">
       <c r="D59" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -2025,7 +2025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5709F210-9363-48A0-87DA-43FC9D18AB36}">
   <dimension ref="A3:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -2580,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>